<commit_message>
Updating the sheet pool names in the bmo unrestricted spreadsheet data.
</commit_message>
<xml_diff>
--- a/app/data/pools/bmo.xlsx
+++ b/app/data/pools/bmo.xlsx
@@ -5,27 +5,27 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="BMO_UR" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="UR Pool 1 - HVAC" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="UR Pool 2 - Plumbing" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="UR Pool 3 - ElevM" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="UR Pool 4 - ElecM" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="UR Pool 5 - Janitorial" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="UR Pool 6 - LndScp" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="UR Pool 7 - FrSysM" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="UR Pool 8 - FrSupr" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="UR Pool 9 - Roof" sheetId="10" state="visible" r:id="rId11"/>
-    <sheet name="UR Pool 10 - BldMgmt" sheetId="11" state="visible" r:id="rId12"/>
-    <sheet name="UR Pool 11 - Archt" sheetId="12" state="visible" r:id="rId13"/>
-    <sheet name="UR Pool 12 - CommSrv" sheetId="13" state="visible" r:id="rId14"/>
-    <sheet name="UR Pool 13 - ElevInsp" sheetId="14" state="visible" r:id="rId15"/>
-    <sheet name="UR Pool 14 - FacMgmt" sheetId="15" state="visible" r:id="rId16"/>
-    <sheet name="UR Pool 15 - Pest" sheetId="16" state="visible" r:id="rId17"/>
-    <sheet name="UR Pool 16 - WstMgmt" sheetId="17" state="visible" r:id="rId18"/>
-    <sheet name="UR Pool 17 - Cemetary" sheetId="18" state="visible" r:id="rId19"/>
+    <sheet name="UR Pool (1) - HVAC" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="UR Pool (2) - Plumbing" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="UR Pool (3) - ElevM" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="UR Pool (4) - ElecM" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="UR Pool (5) - Janitorial" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="UR Pool (6) - LndScp" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="UR Pool (7) - FrSysM" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="UR Pool (8) - FrSupr" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="UR Pool (9) - Roof" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="UR Pool (10) - BldMgmt" sheetId="11" state="visible" r:id="rId12"/>
+    <sheet name="UR Pool (11) - Archt" sheetId="12" state="visible" r:id="rId13"/>
+    <sheet name="UR Pool (12) - CommSrv" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="UR Pool (13) - ElevInsp" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="UR Pool (14) - FacMgmt" sheetId="15" state="visible" r:id="rId16"/>
+    <sheet name="UR Pool (15) - Pest" sheetId="16" state="visible" r:id="rId17"/>
+    <sheet name="UR Pool (16) - WstMgmt" sheetId="17" state="visible" r:id="rId18"/>
+    <sheet name="UR Pool (17) - Cemetary" sheetId="18" state="visible" r:id="rId19"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -557,7 +557,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -579,13 +579,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -699,7 +692,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -723,73 +716,68 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normal 2" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -8031,7 +8019,7 @@
   </sheetPr>
   <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -10299,7 +10287,7 @@
   </sheetPr>
   <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>

</xml_diff>